<commit_message>
Front & back ok
</commit_message>
<xml_diff>
--- a/bd.xlsx
+++ b/bd.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -390,44 +390,69 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="F8" sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>AA</t>
+          <t>Teste Covid</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>2</v>
+        <v>500</v>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Material</t>
+          <t>V. Epidemiológica</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Teste Covid</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VIado</t>
+          <t>Alfinete</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>VIEP</t>
+          <t>CERPAT</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>Teste Covid</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Papel</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>50</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>V. Sanitária</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>Material</t>
         </is>

</xml_diff>